<commit_message>
GPS schematics finished + canbus module start
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E430E7-F55B-4850-92DC-1A4F7644397C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0121530C-668B-4000-87EA-C463AC8E03F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Quantité</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>495-TSR-1-2433</t>
+  </si>
+  <si>
+    <t>1568-1504-ND</t>
+  </si>
+  <si>
+    <t>USB-UART converter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">581-CX3225SB16D0FLJ </t>
+  </si>
+  <si>
+    <t>quartz</t>
   </si>
 </sst>
 </file>
@@ -152,13 +164,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,7 +457,7 @@
   <dimension ref="A8:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,22 +662,22 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I19" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D19" s="2"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I20" s="2">
@@ -713,9 +728,24 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25">
+        <v>14.85</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
       <c r="I25" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.85</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
schematics finished (except gps)
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0121530C-668B-4000-87EA-C463AC8E03F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0F17FE-5B20-4552-BB3D-CD4B75A36943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Quantité</t>
   </si>
@@ -113,6 +113,27 @@
   </si>
   <si>
     <t>quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">871-B82793C104N201 </t>
+  </si>
+  <si>
+    <t>common mode choke</t>
+  </si>
+  <si>
+    <t>497-13262-1-ND</t>
+  </si>
+  <si>
+    <t>diode de protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">495-TCK-141 </t>
+  </si>
+  <si>
+    <t>self</t>
+  </si>
+  <si>
+    <t>296-23759-6-ND</t>
   </si>
 </sst>
 </file>
@@ -457,7 +478,7 @@
   <dimension ref="A8:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +558,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
@@ -553,7 +574,7 @@
       </c>
       <c r="I12" s="2">
         <f>G12*D12</f>
-        <v>2.97</v>
+        <v>8.91</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -671,34 +692,74 @@
       <c r="F18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="2"/>
+      <c r="G18" s="2">
+        <v>1.17</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="0"/>
+        <v>2.0699999999999998</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="2">
+        <v>6.23</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="I20" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.23</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="2"/>
+      <c r="H21" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="I21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="I22" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -711,53 +772,80 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24">
-        <v>1.03</v>
-      </c>
-      <c r="H24" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="0"/>
-        <v>1.03</v>
+        <f>G24*D23</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>1.03</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I25" s="2">
+        <f>G25*D24</f>
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>28</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>14.85</v>
       </c>
-      <c r="H25" t="s">
-        <v>6</v>
-      </c>
-      <c r="I25" s="2">
-        <f t="shared" si="0"/>
-        <v>14.85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>6</v>
+      </c>
       <c r="I26" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G26*D25</f>
+        <v>29.7</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G27">
+        <v>0.41</v>
+      </c>
+      <c r="H27" t="s">
+        <v>6</v>
+      </c>
       <c r="I27" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G27*D26</f>
+        <v>1.23</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
altium project migrated to 4L
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0F17FE-5B20-4552-BB3D-CD4B75A36943}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C870471-C7E9-433D-A916-26CC9371DE67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A8:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>